<commit_message>
Refactoring ETL python packages.
</commit_message>
<xml_diff>
--- a/DataFiles/Source_Data/_ConferenceandTeambyYear.xlsx
+++ b/DataFiles/Source_Data/_ConferenceandTeambyYear.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Home\source\repos\leetroyjenkins\NBADW\DataFiles\Source Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\AppData\Roaming\JetBrains\DataSpell2021.3\projects\NBADW\DataFiles\Source_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E398C1-33A6-4854-B35E-CAC7503291A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A8BBCF-561D-44E8-95A0-EC6A1FD69E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1199,14 +1199,16 @@
   <dimension ref="A1:N441"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K146" sqref="K146"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G124" sqref="G124:G132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -3699,7 +3701,7 @@
       <c r="F124" t="s">
         <v>13</v>
       </c>
-      <c r="G124" t="s">
+      <c r="H124" t="s">
         <v>55</v>
       </c>
       <c r="K124" t="s">
@@ -3725,7 +3727,7 @@
       <c r="F125" t="s">
         <v>62</v>
       </c>
-      <c r="G125" t="s">
+      <c r="H125" t="s">
         <v>25</v>
       </c>
       <c r="K125" t="s">
@@ -3751,7 +3753,7 @@
       <c r="F126" t="s">
         <v>15</v>
       </c>
-      <c r="G126" t="s">
+      <c r="H126" t="s">
         <v>44</v>
       </c>
       <c r="K126" t="s">
@@ -3777,7 +3779,7 @@
       <c r="F127" t="s">
         <v>50</v>
       </c>
-      <c r="G127" t="s">
+      <c r="H127" t="s">
         <v>64</v>
       </c>
       <c r="K127" t="s">
@@ -3820,7 +3822,7 @@
       <c r="F129" t="s">
         <v>13</v>
       </c>
-      <c r="G129" t="s">
+      <c r="H129" t="s">
         <v>55</v>
       </c>
       <c r="K129" t="s">
@@ -3846,7 +3848,7 @@
       <c r="F130" t="s">
         <v>66</v>
       </c>
-      <c r="G130" t="s">
+      <c r="H130" t="s">
         <v>25</v>
       </c>
       <c r="K130" t="s">
@@ -3872,7 +3874,7 @@
       <c r="F131" t="s">
         <v>15</v>
       </c>
-      <c r="G131" t="s">
+      <c r="H131" t="s">
         <v>44</v>
       </c>
       <c r="K131" t="s">
@@ -3898,7 +3900,7 @@
       <c r="F132" t="s">
         <v>50</v>
       </c>
-      <c r="G132" t="s">
+      <c r="H132" t="s">
         <v>68</v>
       </c>
       <c r="K132" t="s">

</xml_diff>